<commit_message>
Added last simulation data
</commit_message>
<xml_diff>
--- a/dataWendy_empty.xlsx
+++ b/dataWendy_empty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId2"/>
@@ -125,8 +125,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,327 +157,327 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>6.17863985336686</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1.23150702065609</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>2.99823031993583</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>7.62169300650492</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>1.37923316795782</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4.31152222398669</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>18.1625852654596</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>3.46583845511892</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>6.33298856182955</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>15.4986648667399</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>3.08130135809995</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>8.82360408292152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>5.16106696562637</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.888476117632255</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>12.2845819089562</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>15.9622034974842</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>3.36202544860985</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>16.9820364830084</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>0.52134812406633</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.102472998228626</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>24.1422658979427</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>17.3189989709467</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>3.51266727352296</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>31.8807482151315</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>9.53019051610425</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>1.94845059557188</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>43.3039949908853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>5.00810089985485</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>0.988942473849189</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>57.2824723538943</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>4.90714595164403</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.946902637612229</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>78.030608355999</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>8.80715434061341</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>1.758392760652</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>103.011687277816</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>2.93019381069867</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.439240213953583</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>136.205732170027</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>2.8168841036999</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.537884406505154</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>179.943538828054</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>6.86522131756397</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>1.29328889142529</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>239.832062782021</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>2.46872225810229</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>0.478560417775372</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>292.268525804859</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>4.79083492089123</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>0.958466051332221</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>369.186416496057</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>5.91226734522303</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>1.12368343769617</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>435.45908310893</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>4.06790321110566</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>0.787937515249327</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>548.213879739866</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>7.81631610152779</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>1.5625562301527</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>648.625092350179</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>1.42127201514417</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>0.285688824656908</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>773.573075808818</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>0.958209260393776</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>0.176007537986191</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>902.198461370077</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>5.61689043656508</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>1.0530757462969</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>1048.74259601603</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>2.88350990772717</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>0.575356564254329</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>1265.65044751903</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>2.64612523818079</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>0.495392287571091</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>1529.31312749092</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>2.05508299542319</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>0.34906100787979</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>1663.4971370569</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>1.00942250280865</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>0.182776867370719</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>2040.75347892288</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>0.533461176887269</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>0.0309227677856495</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>2233.57935741497</v>
       </c>
     </row>
@@ -499,330 +503,330 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>129.518579902669</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>4.50088955467508</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>2.71987285581417</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>82.788157289063</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>3.77592750114961</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>3.93891876912676</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>403.249107467429</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>9.70055793618572</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5.66813126811758</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>300.556197584183</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>8.6216877616594</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>8.0749685219489</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>467.890163890486</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>2.67749984855246</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>11.0263250360731</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>1899.38229477114</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>9.10635690985</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>15.2482332829386</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>16.7832595484001</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.917820857354749</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>22.3637904420029</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>327.955512064629</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>9.84860420450327</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>28.3369601741433</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>133.697086507286</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>5.38511095037071</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>41.3823124580085</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>285.583872384894</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>2.98278467515546</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>57.5465797591023</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>79.8686107604743</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>2.39733103346529</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>78.2949262850452</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>572.618686780298</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>5.26810519279894</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>117.892062223982</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>92.8390916830014</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>1.50493440616715</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>144.830414442113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>44.6731629777553</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>1.42452067950238</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>193.118299086113</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>124.769834462066</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>3.61741399976037</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>229.37832277501</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>46.2017783032818</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>1.18400759082005</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>297.334274743916</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>414.427304183708</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>2.630213347957</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>361.42896133312</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>342.373306080396</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>3.34555531586745</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>441.1673675559</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>165.976430072092</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>2.34590103543321</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>546.619806956034</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>205.247462873121</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>4.35042080599166</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>652.811123946914</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>121.558000803311</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>0.980066742752432</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>718.661229746882</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>115.517911160724</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>0.669722620615015</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>926.365711099002</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>1121.22238834919</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>3.08712553823591</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>1153.84971006587</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>392.46352640843</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>1.5764000622922</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>1211.61026546592</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>98.869071202927</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>1.33950920960133</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>1445.70894940104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>34.9156442098024</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>0.956639177795216</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>1588.13800754002</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>55.5977771301828</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>0.446080898335715</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>1854.08425862202</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>72.7450714412412</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>0.291963146578881</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>2087.36496091308</v>
       </c>
     </row>
@@ -842,34 +846,339 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="n">
+        <v>0.431250312389145</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0.0765267947034013</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>3.54118370916694</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="n">
+        <v>4.41821604890643</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1.7439204836949</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>6.94166351901367</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="n">
+        <v>4.62088010275491</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1.94806913780768</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>8.52647482603788</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="n">
+        <v>2.26850696516621</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.926359078103598</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>16.659964887891</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="n">
+        <v>1.24158654110019</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.470419088310622</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>23.0322765458841</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="n">
+        <v>0.790306240292517</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.320076324341517</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>22.9135151151568</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="n">
+        <v>1.00086294956521</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.373963604375516</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>36.0201362229418</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="n">
+        <v>4.08695665651671</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1.68835465458139</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>53.4192584939301</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="n">
+        <v>1.39650800133352</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0.578800879008363</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>64.5396408140659</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="n">
+        <v>1.22675354326406</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0.489713266141264</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>81.3643256558571</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="n">
+        <v>0.690101184598249</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0.270048855626893</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>108.060310218018</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="n">
+        <v>0.161505404840646</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0.0249628370881521</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>117.775018518092</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="n">
+        <v>0.872094848129713</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0.343697820527174</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>160.611993290018</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="n">
+        <v>1.29431134366567</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0.525345745886366</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>198.808485885151</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="n">
+        <v>1.34281246545854</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0.55010683284486</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>240.306651290972</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="n">
+        <v>0.17511733056277</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0.0553639313545437</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>263.940323393093</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="n">
+        <v>1.22725025484002</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0.49070012994122</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>345.002666122979</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="n">
+        <v>0.288261755530378</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>0.116479178890817</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>424.926923917141</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="n">
+        <v>0.402434525077644</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0.153043852840032</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>486.247570659965</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1" t="n">
+        <v>0.267053361716556</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0.0811703332341553</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>604.912980695022</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="1" t="n">
+        <v>0.786158230522531</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>0.332242309864351</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>654.744497881038</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="n">
+        <v>0.64667990284274</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0.257679089506259</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>837.432177310111</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="n">
+        <v>0.610558569268778</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0.246282238996382</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>960.039072556188</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="n">
+        <v>0.680845706012189</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>0.279098491672707</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1142.20078309206</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="n">
+        <v>0.845411449440641</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>0.346253653342079</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1305.23401854001</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="n">
+        <v>1.19365303825851</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>0.493210882099176</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1519.16465058899</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="n">
+        <v>0.455340671419922</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>0.182268529425019</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>1878.82989552082</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="1" t="n">
+        <v>0.285627500576386</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0.111332835543833</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>2197.63818161096</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -888,332 +1197,332 @@
   </sheetPr>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="n">
-        <v>6.17863985336686</v>
+        <v>1.08835106915168</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1.23150702065609</v>
+        <v>0.741263295480547</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>2.99823031993583</v>
+        <v>3.16692306799814</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
-        <v>7.62169300650492</v>
+        <v>1.32779487966806</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1.37923316795782</v>
+        <v>0.8868943826136</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>4.31152222398669</v>
+        <v>4.6424187629018</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
-        <v>18.1625852654596</v>
+        <v>2.85441174608052</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3.46583845511892</v>
+        <v>1.92942119463162</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>6.33298856182955</v>
+        <v>6.6817441477906</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
-        <v>15.4986648667399</v>
+        <v>3.2619170076856</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>3.08130135809995</v>
+        <v>2.17934175588669</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>8.82360408292152</v>
+        <v>10.1318455468863</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
-        <v>5.16106696562637</v>
+        <v>0.7478832784849</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.888476117632255</v>
+        <v>0.448352534007569</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>12.2845819089562</v>
+        <v>13.8348186288495</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
-        <v>15.9622034974842</v>
+        <v>3.37071568973793</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>3.36202544860985</v>
+        <v>2.24711380914067</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>16.9820364830084</v>
+        <v>21.4339436769951</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
-        <v>0.52134812406633</v>
+        <v>0.179170478968964</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.102472998228626</v>
+        <v>0.0786534455962349</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>24.1422658979427</v>
+        <v>28.9510978991166</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
-        <v>17.3189989709467</v>
+        <v>2.92482678355509</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>3.51266727352296</v>
+        <v>1.97524680505348</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>31.8807482151315</v>
+        <v>42.9089314718731</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
-        <v>9.53019051610425</v>
+        <v>2.00314086783124</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>1.94845059557188</v>
+        <v>1.34296793565419</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>43.3039949908853</v>
+        <v>63.1176811438054</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
-        <v>5.00810089985485</v>
+        <v>0.777687713648376</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0.988942473849189</v>
+        <v>0.521806252359637</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>57.2824723538943</v>
+        <v>84.4061999118421</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
-        <v>4.90714595164403</v>
+        <v>0.879504173458756</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0.946902637612229</v>
+        <v>0.586648729328877</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>78.030608355999</v>
+        <v>111.468337440863</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
-        <v>8.80715434061341</v>
+        <v>1.52704656213998</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>1.758392760652</v>
+        <v>1.02946906971309</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>103.011687277816</v>
+        <v>145.935725651914</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
-        <v>2.93019381069867</v>
+        <v>0.466680598226237</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0.439240213953583</v>
+        <v>0.234250204318935</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>136.205732170027</v>
+        <v>167.173644499155</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
-        <v>2.8168841036999</v>
+        <v>0.559333523719816</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0.537884406505154</v>
+        <v>0.375566253879983</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>179.943538828054</v>
+        <v>220.772209327202</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
-        <v>6.86522131756397</v>
+        <v>1.25426254265676</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>1.29328889142529</v>
+        <v>0.839534132413482</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>239.832062782021</v>
+        <v>284.684503606986</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
-        <v>2.46872225810229</v>
+        <v>0.463869115321428</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.478560417775372</v>
+        <v>0.310524560936149</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>292.268525804859</v>
+        <v>337.496438192902</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
-        <v>4.79083492089123</v>
+        <v>0.904389447250382</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.958466051332221</v>
+        <v>0.605820957500016</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>369.186416496057</v>
+        <v>406.153980594128</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
-        <v>5.91226734522303</v>
+        <v>0.983721718297886</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>1.12368343769617</v>
+        <v>0.661037300463642</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>435.45908310893</v>
+        <v>496.69494201499</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
-        <v>4.06790321110566</v>
+        <v>0.653494263983001</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0.787937515249327</v>
+        <v>0.438201268837146</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>548.213879739866</v>
+        <v>596.803548413096</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
-        <v>7.81631610152779</v>
+        <v>1.5053218721455</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>1.5625562301527</v>
+        <v>1.00775296291955</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>648.625092350179</v>
+        <v>736.554291390115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
-        <v>1.42127201514417</v>
+        <v>0.24736438692217</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>0.285688824656908</v>
+        <v>0.1645199411717</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>773.573075808818</v>
+        <v>797.849416601006</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
-        <v>0.958209260393776</v>
+        <v>0.162126941859709</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0.176007537986191</v>
+        <v>0.105601510895479</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>902.198461370077</v>
+        <v>997.069913156796</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
-        <v>5.61689043656508</v>
+        <v>0.913808783302607</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>1.0530757462969</v>
+        <v>0.612972206141261</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>1048.74259601603</v>
+        <v>1102.18297168403</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="n">
-        <v>2.88350990772717</v>
+        <v>0.568337123584106</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>0.575356564254329</v>
+        <v>0.38165146317532</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>1265.65044751903</v>
+        <v>1337.40452689189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="n">
-        <v>2.64612523818079</v>
+        <v>0.47130273716788</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>0.495392287571091</v>
+        <v>0.315220657723485</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>1529.31312749092</v>
+        <v>1554.51312229293</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="n">
-        <v>2.05508299542319</v>
+        <v>0.334709509410423</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>0.34906100787979</v>
+        <v>0.223802103789153</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1663.4971370569</v>
+        <v>1802.86937115318</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
-        <v>1.00942250280865</v>
+        <v>0.191872490971408</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>0.182776867370719</v>
+        <v>0.117063909322988</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>2040.75347892288</v>
+        <v>2094.77226911695</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="n">
-        <v>0.533461176887269</v>
+        <v>0.135765454596867</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>0.0309227677856495</v>
+        <v>0.00700652683122687</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>2233.57935741497</v>
+        <v>2351.31391827203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>